<commit_message>
Started building out some of the NFA and DFA routines for the parser(s)
Signed-off-by: duncanamps <duncan@duncanamps.com>
</commit_message>
<xml_diff>
--- a/docs/command_line.xlsx
+++ b/docs/command_line.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Duncan Munro\Dropbox\dev\lazarus\computing\z80\xa80\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63282087-1D66-46AC-999E-5178E2C9F859}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD4AEFAB-56BD-4991-97CA-49C8D6A741D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2688" yWindow="408" windowWidth="20004" windowHeight="11832" xr2:uid="{5CD26827-941F-4AA0-9E70-4501816D361F}"/>
   </bookViews>
@@ -178,17 +178,19 @@
     <t>-s &lt;topic&gt;</t>
   </si>
   <si>
-    <t>--show &lt;topic&gt;</t>
-  </si>
-  <si>
     <t>Show information on a range of topics:
-•	distribution – the licence rules on distributing the software
-•	grammar – the full list of grammar rules being applied
-•	instructions – the full list of instructions available
-•	operators – the operators which are used and their priority
-•	reserved – the reserved words used for the chosen processor and grammar
-•	version – the version of the software and other key details
-•	warranty – the warranty available with the software</t>
+• dfa – the Deterministic Finite Automata for the expression parser
+• distribution – the licence rules on distributing the software
+• grammar – the full list of grammar rules being applied
+• instructions – the full list of instructions available
+• nfa – the Non-deterministic Finite Automata for the expression parser
+• operators – the operators which are used and their priority
+• reserved – the reserved words used for the chosen processor and grammar
+• version – the version of the software and other key details
+• warranty – the warranty available with the software</t>
+  </si>
+  <si>
+    <t>--show=&lt;topic&gt;</t>
   </si>
 </sst>
 </file>
@@ -601,9 +603,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58DEEA83-DD36-4C3F-AE5D-DFA228A2A034}">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -824,18 +824,18 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>46</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>40</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
Start of major rebuild for V0.2
Signed-off-by: duncanamps <duncan@duncanamps.com>
</commit_message>
<xml_diff>
--- a/docs/command_line.xlsx
+++ b/docs/command_line.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Duncan Munro\Dropbox\dev\lazarus\computing\z80\xa80\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD4AEFAB-56BD-4991-97CA-49C8D6A741D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4768ED9-3A15-4A82-B44E-E74318747ED2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="408" windowWidth="20004" windowHeight="11832" xr2:uid="{5CD26827-941F-4AA0-9E70-4501816D361F}"/>
+    <workbookView xWindow="1920" yWindow="408" windowWidth="20004" windowHeight="11832" xr2:uid="{5CD26827-941F-4AA0-9E70-4501816D361F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="58">
   <si>
     <t>Switch</t>
   </si>
@@ -55,9 +55,6 @@
     <t>--debug=&lt;bn&gt;</t>
   </si>
   <si>
-    <t>Set the debug filename to &lt;bn&gt;. If a file extension is not specified, then a default of .dbg80 is used. If &lt;bn&gt; is not specified, the filename is the assembler file name with the filetype changed to .dbg80. If this switch is not present, no debug file is produced</t>
-  </si>
-  <si>
     <t>No</t>
   </si>
   <si>
@@ -94,27 +91,18 @@
     <t>--listing=&lt;ln&gt;</t>
   </si>
   <si>
-    <t>Sets the listing filename to &lt;ln&gt;. If a file extension is not specified then a default of .lst is used. If &lt;ln&gt; is not specified, the filename is the assembler file name with the filetype changed to .lst. If this switch is not present, no listing file is produced</t>
-  </si>
-  <si>
     <t>-m &lt;mn&gt;</t>
   </si>
   <si>
     <t>--map=&lt;mn&gt;</t>
   </si>
   <si>
-    <t>Sets the map filename to &lt;mn&gt;. If a file extension is not specified then a default of .map is used. If &lt;mn&gt; is not specified, the filename is the assembler file name with the filetype changed to .map. If this switch is not present, no map file is produced</t>
-  </si>
-  <si>
     <t>-o &lt;on&gt;</t>
   </si>
   <si>
     <t>--object=&lt;on&gt;</t>
   </si>
   <si>
-    <t>Set the object filename to &lt;on&gt;. If a file extension is not specified then a default of .obj80 is used. If &lt;on&gt; is not specified, the filename is the assembler file name with the filetype changed to .obj80. If this switch is not present, no object file is produced</t>
-  </si>
-  <si>
     <t>-p &lt;pt&gt;</t>
   </si>
   <si>
@@ -145,12 +133,6 @@
     <t>Command line switches</t>
   </si>
   <si>
-    <t>Verbose output when assembling. Values are: 0. Normal level (default), 1. Verbose output, 2. War and Peace with lots more output, 3. Debug level. The debug level is only relevant with Debug versions of the software</t>
-  </si>
-  <si>
-    <t>Set the hex filename to &lt;hn&gt;. If a file extension is not specified then a default of .hex is used. If &lt;hn&gt; is not specified, the filename is the assembler file name with the filetype changed to .hex. If this switch is not present, no hex file is produced</t>
-  </si>
-  <si>
     <t>Parameter</t>
   </si>
   <si>
@@ -178,19 +160,72 @@
     <t>-s &lt;topic&gt;</t>
   </si>
   <si>
+    <t>--show=&lt;topic&gt;</t>
+  </si>
+  <si>
+    <t>Set the debug filename or folder to &lt;bn&gt;. If a file extension is not specified, then a default of .dbg80 is used. If &lt;bn&gt; is not specified, the filename is the assembler file name with the filetype changed to .dbg80. If this switch is not present, no debug file is produced</t>
+  </si>
+  <si>
+    <t>Sets the listing filename or folder to &lt;ln&gt;. If a file extension is not specified then a default of .lst is used. If &lt;ln&gt; is not specified, the filename is the assembler file name with the filetype changed to .lst. If this switch is not present, no listing file is produced</t>
+  </si>
+  <si>
+    <t>Sets the map filename or folder to &lt;mn&gt;. If a file extension is not specified then a default of .map is used. If &lt;mn&gt; is not specified, the filename is the assembler file name with the filetype changed to .map. If this switch is not present, no map file is produced</t>
+  </si>
+  <si>
+    <t>Set the object filename or folder to &lt;on&gt;. If a file extension is not specified then a default of .obj80 is used. If &lt;on&gt; is not specified, the filename is the assembler file name with the filetype changed to .obj80. If this switch is not present, no object file is produced</t>
+  </si>
+  <si>
+    <t>Set the hex filename or folder to &lt;hn&gt;. If a file extension is not specified then a default of .hex is used. If &lt;hn&gt; is not specified, the filename is the assembler file name with the filetype changed to .hex. If this switch is not present, no hex file is produced</t>
+  </si>
+  <si>
+    <t>Verbose output when assembling. Values are:
+0. Silent - only shows fatal and internal errors
+1. Normal level (default)
+2. Verbose output
+3. War and Peace with lots more output
+4. Debug level. The debug level is only relevant with Debug versions of the software</t>
+  </si>
+  <si>
+    <t>-c &lt;cn&gt;</t>
+  </si>
+  <si>
+    <t>--com=&lt;cn&gt;</t>
+  </si>
+  <si>
+    <t>Set the .com/.bin filename or folder to &lt;cn&gt;. If a file extension is not specified, then a default of .com is used. If &lt;cn&gt; is not specified, the filename is the assembler file name with the filetype changed to .com. If this switch is not present, no binary file is produced</t>
+  </si>
+  <si>
+    <t>-e &lt;en&gt;</t>
+  </si>
+  <si>
+    <t>--errorlog=&lt;en&gt;</t>
+  </si>
+  <si>
+    <t>Set the error log filename or folder to &lt;en&gt;. If a file extension is not specified, then a default of .log is used. If &lt;en&gt; is not specified, the filename is the assembler file name with the filetype changed to .log. If this switch is not present, no error log file is produced</t>
+  </si>
+  <si>
+    <t>-d &lt;id&gt;</t>
+  </si>
+  <si>
+    <t>--define=&lt;id&gt;</t>
+  </si>
+  <si>
+    <t>Creates defines in the symbol table for the items represented by &lt;id&gt;. This can be a symbol name or a numeric or a string value, for example --define=DEBUG. It's possible to have multiple entries separated by semicolons, e.g. --define=DEBUG;ARRAYS=5;TITLE="My Prog"</t>
+  </si>
+  <si>
     <t>Show information on a range of topics:
-• dfa – the Deterministic Finite Automata for the expression parser
+• dfae – the Deterministic Finite Automata for the expression parser
+• dfap – the Deterministic Finite Automata for the pre-parser
 • distribution – the licence rules on distributing the software
+• environment – the environment for the assembler
 • grammar – the full list of grammar rules being applied
 • instructions – the full list of instructions available
-• nfa – the Non-deterministic Finite Automata for the expression parser
+• nfae – the Non-deterministic Finite Automata for the expression parser
+• nfap – the Non-deterministic Finite Automata for the pre-parser
 • operators – the operators which are used and their priority
 • reserved – the reserved words used for the chosen processor and grammar
 • version – the version of the software and other key details
 • warranty – the warranty available with the software</t>
-  </si>
-  <si>
-    <t>--show=&lt;topic&gt;</t>
   </si>
 </sst>
 </file>
@@ -289,8 +324,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F072B5D0-AFA6-4C8B-B0C9-51DD6EC0E4A5}" name="Table1" displayName="Table1" ref="A3:G15" totalsRowShown="0" dataDxfId="7">
-  <autoFilter ref="A3:G15" xr:uid="{F072B5D0-AFA6-4C8B-B0C9-51DD6EC0E4A5}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F072B5D0-AFA6-4C8B-B0C9-51DD6EC0E4A5}" name="Table1" displayName="Table1" ref="A3:G18" totalsRowShown="0" dataDxfId="7">
+  <autoFilter ref="A3:G18" xr:uid="{F072B5D0-AFA6-4C8B-B0C9-51DD6EC0E4A5}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{EFEC94ED-8610-4B46-9BE3-80608EBBD7AA}" name="Switch" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{33D4DCCF-D41A-475F-93EF-2059A2FFA2C8}" name="Long form" dataDxfId="5"/>
@@ -601,9 +636,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58DEEA83-DD36-4C3F-AE5D-DFA228A2A034}">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -614,7 +651,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -625,7 +662,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="D3" t="s">
         <v>2</v>
@@ -634,10 +671,10 @@
         <v>3</v>
       </c>
       <c r="F3" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="G3" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="72" x14ac:dyDescent="0.3">
@@ -648,272 +685,341 @@
         <v>5</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>6</v>
+        <v>42</v>
       </c>
       <c r="E4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="B8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+      <c r="B9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C9" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D6" s="3" t="s">
+      <c r="E9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+      <c r="B10" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="C10" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D7" s="3" t="s">
+      <c r="E10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="72" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+      <c r="B11" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="72" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="72" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="C11" s="2" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>43</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="230.4" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="302.39999999999998" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D18" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="72" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>7</v>
+      <c r="E18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>